<commit_message>
Mejorara de la interfaz de usuario adaptable y la selección predeterminada para los reportes
Se agregó un menú desplegable adaptable para la navegación móvil en la página de inicio, se mejoraron el diseño y los controles del componente Pozos para una mejor experiencia en dispositivos móviles y de escritorio, se estableció la conexión predeterminada a "Poza Rica" y se actualizó la lógica de carga de datos. También se eliminó un favicon sin usar y se actualizó la plantilla de informe diario.
</commit_message>
<xml_diff>
--- a/public/plantillaReporteDiario.xlsx
+++ b/public/plantillaReporteDiario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ismae\OneDrive\Escritorio\Reporteador\Frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845C21AD-1307-422B-B954-38414038E8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AB8A72-4CEC-4E7A-8D29-4B51AE175BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{11315CA4-D2DE-451E-A7A8-FF9D3E544B73}"/>
   </bookViews>
@@ -33,6 +33,38 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+  </valueMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,7 +452,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -497,10 +529,46 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="11" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -512,42 +580,14 @@
     <xf numFmtId="14" fontId="11" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,203 +607,79 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>23376</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>23375</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>185854</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 0" descr="65adb373-c27c-46ae-a553-68d93f73d70f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0349E4FD-BB4E-4953-ACFB-582AD5460968}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7315716" y="8199635"/>
-          <a:ext cx="2735064" cy="756839"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>11759</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>11760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 0" descr="65adb373-c27c-46ae-a553-68d93f73d70f">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BF26693-5674-4AB2-AB1A-2151E1716CD1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7304099" y="240360"/>
-          <a:ext cx="2746681" cy="780720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>624841</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>547</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagen 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B15669EC-475F-47DC-8341-0CC9C5184C0E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect l="13690" t="25714" r="16605" b="23810"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1" y="236221"/>
-          <a:ext cx="2430780" cy="914946"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>233842</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>54712</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>39584</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagen 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72C16B65-CB53-4532-8A1D-3CF5F481154F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect l="13690" t="25714" r="16605" b="23810"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="8012180"/>
-          <a:ext cx="2529109" cy="755768"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="1">
+    <v>1</v>
+    <v>5</v>
+    <v>65adb373-c27c-46ae-a553-68d93f73d70f</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+    <k n="Text" t="s"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1085,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86FA0F4-6A84-44E9-BF44-DE33A70EE4B7}">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="77" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,96 +1011,128 @@
     <col min="2" max="7" width="10" customWidth="1"/>
     <col min="8" max="10" width="10" style="2" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="12" max="13" width="15.109375" customWidth="1"/>
-    <col min="14" max="42" width="10" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" customWidth="1"/>
+    <col min="14" max="14" width="2.33203125" hidden="1" customWidth="1"/>
+    <col min="15" max="42" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D1" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
+      <c r="D1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D3" s="35" t="s">
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D4" s="35" t="s">
+      <c r="A4" s="34" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D5" s="35" t="s">
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="51" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+    </row>
+    <row r="5" spans="1:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D6" s="35" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45" t="s">
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="L8" s="46" t="s">
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="L8" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="46" t="s">
+      <c r="M8" s="44" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="46" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1214,11 +1162,11 @@
       <c r="J9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
@@ -2277,14 +2225,14 @@
       <c r="N40" s="29"/>
     </row>
     <row r="41" spans="1:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D41" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
-      <c r="I41" s="50"/>
+      <c r="D41" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
       <c r="J41" s="1"/>
       <c r="M41" s="30"/>
       <c r="O41" s="30"/>
@@ -2294,48 +2242,73 @@
       <c r="S41" s="29"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D42" s="34" t="str">
+      <c r="A42" s="34" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="36" t="str">
         <f>+D2</f>
         <v xml:space="preserve">Coordinación de Operación De Explotación </v>
       </c>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="36"/>
+      <c r="K42" s="51" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L42" s="51"/>
+      <c r="M42" s="51"/>
+      <c r="N42" s="53"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D43" s="35" t="str">
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34" t="str">
         <f>+D3</f>
         <v>Contrato 425014809</v>
       </c>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D44" s="35" t="str">
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="K43" s="51"/>
+      <c r="L43" s="51"/>
+      <c r="M43" s="51"/>
+      <c r="N43" s="53"/>
+    </row>
+    <row r="44" spans="1:19" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="52" t="str">
         <f>+D4</f>
         <v>Pozo IRIDE 5108</v>
       </c>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="51"/>
+      <c r="M44" s="51"/>
+      <c r="N44" s="53"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D45" s="35" t="str">
+      <c r="D45" s="34" t="str">
         <f>+D5</f>
         <v>Supervisor Ing. Angel Adrian Castro Acosta.</v>
       </c>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
     </row>
     <row r="46" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E46" t="str">
@@ -2344,50 +2317,50 @@
       </c>
     </row>
     <row r="47" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="37"/>
-      <c r="L47" s="38"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="49"/>
+      <c r="K47" s="49"/>
+      <c r="L47" s="50"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="40"/>
-      <c r="J48" s="40"/>
-      <c r="K48" s="40"/>
-      <c r="L48" s="41"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="38"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="39"/>
     </row>
     <row r="49" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="42"/>
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="44"/>
+      <c r="A49" s="40"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="41"/>
+      <c r="K49" s="41"/>
+      <c r="L49" s="42"/>
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="31"/>
@@ -2406,13 +2379,11 @@
     <row r="51" spans="1:12" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D5:I5"/>
+  <mergeCells count="22">
+    <mergeCell ref="A42:C44"/>
+    <mergeCell ref="K4:M6"/>
+    <mergeCell ref="K42:M44"/>
+    <mergeCell ref="A4:C6"/>
     <mergeCell ref="A48:L49"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="F8:J8"/>
@@ -2425,8 +2396,13 @@
     <mergeCell ref="D44:I44"/>
     <mergeCell ref="D45:I45"/>
     <mergeCell ref="A47:L47"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mejoras en pozos y reporte: filtros, gráficos y conexiones
Se agregan filtros por nombre en la tabla de pozos, se mejora la gestión y persistencia de la conexión seleccionada, y se optimiza la carga de datos con debounce y cache. En el reporte, se añade el campo Qiny, se actualiza la plantilla Excel y se generan tres gráficos automáticos (gráficos 8, 9 y 12) en la exportación. Se actualizan nombres de conexiones y se mejora la experiencia de usuario al mostrar el nombre del activo de extracción en el reporte.
</commit_message>
<xml_diff>
--- a/public/plantillaReporteDiario.xlsx
+++ b/public/plantillaReporteDiario.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ismae\OneDrive\Escritorio\Reporteador\Frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AB8A72-4CEC-4E7A-8D29-4B51AE175BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A01AFA-B50F-4194-8BE2-DFEDD88E8BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{11315CA4-D2DE-451E-A7A8-FF9D3E544B73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -293,7 +296,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -446,6 +449,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -474,9 +486,6 @@
     <xf numFmtId="166" fontId="6" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -529,6 +538,15 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -538,6 +556,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -580,14 +604,6 @@
     <xf numFmtId="14" fontId="11" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,6 +621,532 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="SAM 1199"/>
+      <sheetName val="IRIDE 5108"/>
+      <sheetName val="SAMARIA 91A"/>
+      <sheetName val="SAMARIA 7122"/>
+      <sheetName val="SAMARIA 76(B)"/>
+      <sheetName val="SAMARIA 7107"/>
+      <sheetName val="SAMARIA 6093"/>
+      <sheetName val="SAMARIA 6102"/>
+      <sheetName val="SAMARIA 102-A"/>
+      <sheetName val="SAMARIA 7192"/>
+      <sheetName val="SAMARIA 6075"/>
+      <sheetName val="SAMARIA 6092-H"/>
+      <sheetName val="SAMARIA 5111"/>
+      <sheetName val="SAMARIA 4112"/>
+      <sheetName val="SAMARIA 1075"/>
+      <sheetName val="CUNDUACAN 10"/>
+      <sheetName val="SAMARIA 5104"/>
+      <sheetName val="SAMARIA 1081"/>
+      <sheetName val="SAMARIA 5084"/>
+      <sheetName val="SAMARIA 71"/>
+      <sheetName val="SAMARIA 7011"/>
+      <sheetName val="SAMARIA 7114-H "/>
+      <sheetName val="SAMARIA 7076"/>
+      <sheetName val="SAMARIA 73-A"/>
+      <sheetName val="SAMARIA 5199"/>
+      <sheetName val="SAMARIA 6084"/>
+      <sheetName val="M. CUNDUACAN 21"/>
+      <sheetName val="M. SAMARIA 5081"/>
+      <sheetName val="M. IRIDE 1126"/>
+      <sheetName val="M. OXIACAQUE 13"/>
+      <sheetName val="M. OXIACAQUE 26"/>
+      <sheetName val="M. CUNDUACAN 25"/>
+      <sheetName val="M. CUNDUACAN 1"/>
+      <sheetName val="M. SAMARIA 1187"/>
+      <sheetName val="M.CUNDUACAN 10"/>
+      <sheetName val="M. SAMARIA 82"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="8">
+          <cell r="M8" t="str">
+            <v>Q iny</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>TP</v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>TR</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>LDD</v>
+          </cell>
+          <cell r="M9"/>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>kg/cm2</v>
+          </cell>
+          <cell r="C10" t="str">
+            <v>kg/cm2</v>
+          </cell>
+          <cell r="D10" t="str">
+            <v>kg/cm2</v>
+          </cell>
+          <cell r="M10" t="str">
+            <v>MMPCD</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>12.98</v>
+          </cell>
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+          <cell r="D11">
+            <v>10.92</v>
+          </cell>
+          <cell r="L11">
+            <v>6</v>
+          </cell>
+          <cell r="M11">
+            <v>2.5099999999999998</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>27.25</v>
+          </cell>
+          <cell r="C12">
+            <v>0</v>
+          </cell>
+          <cell r="D12">
+            <v>26.42</v>
+          </cell>
+          <cell r="L12">
+            <v>7</v>
+          </cell>
+          <cell r="M12">
+            <v>2.5</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>11.86</v>
+          </cell>
+          <cell r="C13">
+            <v>0</v>
+          </cell>
+          <cell r="D13">
+            <v>11.54</v>
+          </cell>
+          <cell r="L13">
+            <v>8</v>
+          </cell>
+          <cell r="M13">
+            <v>2.5099999999999998</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14">
+            <v>9.6999999999999993</v>
+          </cell>
+          <cell r="C14">
+            <v>0</v>
+          </cell>
+          <cell r="D14">
+            <v>8.86</v>
+          </cell>
+          <cell r="L14">
+            <v>9</v>
+          </cell>
+          <cell r="M14">
+            <v>2.48</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15">
+            <v>11.39</v>
+          </cell>
+          <cell r="C15">
+            <v>0</v>
+          </cell>
+          <cell r="D15">
+            <v>10.08</v>
+          </cell>
+          <cell r="L15">
+            <v>10</v>
+          </cell>
+          <cell r="M15">
+            <v>2.5099999999999998</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16">
+            <v>21.07</v>
+          </cell>
+          <cell r="C16">
+            <v>0</v>
+          </cell>
+          <cell r="D16">
+            <v>17.64</v>
+          </cell>
+          <cell r="L16">
+            <v>11</v>
+          </cell>
+          <cell r="M16">
+            <v>2.52</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17">
+            <v>20.239999999999998</v>
+          </cell>
+          <cell r="C17">
+            <v>0</v>
+          </cell>
+          <cell r="D17">
+            <v>19.5</v>
+          </cell>
+          <cell r="L17">
+            <v>12</v>
+          </cell>
+          <cell r="M17">
+            <v>2.5099999999999998</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18">
+            <v>10.16</v>
+          </cell>
+          <cell r="C18">
+            <v>0</v>
+          </cell>
+          <cell r="D18">
+            <v>9.07</v>
+          </cell>
+          <cell r="L18">
+            <v>13</v>
+          </cell>
+          <cell r="M18">
+            <v>2.4500000000000002</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19">
+            <v>9.31</v>
+          </cell>
+          <cell r="C19">
+            <v>0</v>
+          </cell>
+          <cell r="D19">
+            <v>8.6199999999999992</v>
+          </cell>
+          <cell r="L19">
+            <v>14</v>
+          </cell>
+          <cell r="M19">
+            <v>2.46</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="B20">
+            <v>13.64</v>
+          </cell>
+          <cell r="C20">
+            <v>0</v>
+          </cell>
+          <cell r="D20">
+            <v>11.63</v>
+          </cell>
+          <cell r="L20">
+            <v>15</v>
+          </cell>
+          <cell r="M20">
+            <v>2.4700000000000002</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="B21">
+            <v>26.07</v>
+          </cell>
+          <cell r="C21">
+            <v>0</v>
+          </cell>
+          <cell r="D21">
+            <v>23.83</v>
+          </cell>
+          <cell r="L21">
+            <v>16</v>
+          </cell>
+          <cell r="M21">
+            <v>2.4500000000000002</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22">
+            <v>12.09</v>
+          </cell>
+          <cell r="C22">
+            <v>0</v>
+          </cell>
+          <cell r="D22">
+            <v>11.09</v>
+          </cell>
+          <cell r="L22">
+            <v>17</v>
+          </cell>
+          <cell r="M22">
+            <v>2.5499999999999998</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23">
+            <v>10.56</v>
+          </cell>
+          <cell r="C23">
+            <v>0</v>
+          </cell>
+          <cell r="D23">
+            <v>9.31</v>
+          </cell>
+          <cell r="L23">
+            <v>18</v>
+          </cell>
+          <cell r="M23">
+            <v>2.62</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24">
+            <v>12.33</v>
+          </cell>
+          <cell r="C24">
+            <v>0</v>
+          </cell>
+          <cell r="D24">
+            <v>10.43</v>
+          </cell>
+          <cell r="L24">
+            <v>19</v>
+          </cell>
+          <cell r="M24">
+            <v>2.6</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25">
+            <v>25.29</v>
+          </cell>
+          <cell r="C25">
+            <v>0</v>
+          </cell>
+          <cell r="D25">
+            <v>23.56</v>
+          </cell>
+          <cell r="L25">
+            <v>20</v>
+          </cell>
+          <cell r="M25">
+            <v>2.62</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="B26">
+            <v>14.51</v>
+          </cell>
+          <cell r="C26">
+            <v>0</v>
+          </cell>
+          <cell r="D26">
+            <v>14.23</v>
+          </cell>
+          <cell r="L26">
+            <v>21</v>
+          </cell>
+          <cell r="M26">
+            <v>2.62</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="B27">
+            <v>10.44</v>
+          </cell>
+          <cell r="C27">
+            <v>0</v>
+          </cell>
+          <cell r="D27">
+            <v>9.2200000000000006</v>
+          </cell>
+          <cell r="L27">
+            <v>22</v>
+          </cell>
+          <cell r="M27">
+            <v>2.61</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28">
+            <v>11.31</v>
+          </cell>
+          <cell r="C28">
+            <v>0</v>
+          </cell>
+          <cell r="D28">
+            <v>9.6</v>
+          </cell>
+          <cell r="L28">
+            <v>23</v>
+          </cell>
+          <cell r="M28">
+            <v>2.61</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29">
+            <v>24.12</v>
+          </cell>
+          <cell r="C29">
+            <v>0</v>
+          </cell>
+          <cell r="D29">
+            <v>22.17</v>
+          </cell>
+          <cell r="L29">
+            <v>0</v>
+          </cell>
+          <cell r="M29">
+            <v>2.62</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="B30">
+            <v>15.81</v>
+          </cell>
+          <cell r="C30">
+            <v>0</v>
+          </cell>
+          <cell r="D30">
+            <v>15.12</v>
+          </cell>
+          <cell r="L30">
+            <v>1</v>
+          </cell>
+          <cell r="M30">
+            <v>2.62</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="B31">
+            <v>10.26</v>
+          </cell>
+          <cell r="C31">
+            <v>0</v>
+          </cell>
+          <cell r="D31">
+            <v>9.0399999999999991</v>
+          </cell>
+          <cell r="L31">
+            <v>2</v>
+          </cell>
+          <cell r="M31">
+            <v>2.61</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="B32">
+            <v>10.09</v>
+          </cell>
+          <cell r="C32">
+            <v>0</v>
+          </cell>
+          <cell r="D32">
+            <v>8.8800000000000008</v>
+          </cell>
+          <cell r="L32">
+            <v>3</v>
+          </cell>
+          <cell r="M32">
+            <v>2.62</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="B33">
+            <v>19.87</v>
+          </cell>
+          <cell r="C33">
+            <v>0</v>
+          </cell>
+          <cell r="D33">
+            <v>16.559999999999999</v>
+          </cell>
+          <cell r="L33">
+            <v>4</v>
+          </cell>
+          <cell r="M33">
+            <v>2.62</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="B34">
+            <v>28.16</v>
+          </cell>
+          <cell r="C34">
+            <v>0</v>
+          </cell>
+          <cell r="D34">
+            <v>27.4</v>
+          </cell>
+          <cell r="L34">
+            <v>5</v>
+          </cell>
+          <cell r="M34">
+            <v>2.62</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1001,8 +1543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86FA0F4-6A84-44E9-BF44-DE33A70EE4B7}">
   <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1018,121 +1560,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="e" vm="1">
+      <c r="A4" s="36" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="51" t="e" vm="2">
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="K4" s="40" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
     </row>
     <row r="5" spans="1:14" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="52" t="s">
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34" t="s">
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="51"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43" t="s">
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="L8" s="44" t="s">
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="L8" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="44" t="s">
+      <c r="M8" s="48" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="50" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1162,11 +1698,11 @@
       <c r="J9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="47"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
@@ -1206,1180 +1742,1233 @@
         <v>10</v>
       </c>
       <c r="B11" s="8">
+        <v>2</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>2</v>
+      </c>
+      <c r="E11" s="8">
+        <v>2</v>
+      </c>
+      <c r="F11" s="8">
+        <v>2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>10</v>
+      </c>
+      <c r="H11" s="8">
+        <v>2</v>
+      </c>
+      <c r="I11" s="8">
+        <v>2</v>
+      </c>
+      <c r="J11" s="8">
+        <v>2</v>
+      </c>
+      <c r="L11" s="33">
         <v>0</v>
       </c>
-      <c r="C11" s="8">
-        <v>0</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0</v>
-      </c>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-      <c r="H11" s="8">
-        <v>0</v>
-      </c>
-      <c r="I11" s="8">
-        <v>0</v>
-      </c>
-      <c r="J11" s="8">
-        <v>0</v>
-      </c>
-      <c r="L11" s="9"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="11"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C12" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D12" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E12" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F12" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G12" s="8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H12" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I12" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J12" s="8">
-        <v>0</v>
-      </c>
-      <c r="L12" s="9"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="L12" s="34">
+        <v>1</v>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C13" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D13" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E13" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F13" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G13" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H13" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I13" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="L13" s="33">
+        <v>2</v>
+      </c>
+      <c r="M13" s="9"/>
+      <c r="N13" s="10"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C14" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D14" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E14" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F14" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G14" s="8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H14" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I14" s="8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J14" s="8">
-        <v>0</v>
-      </c>
-      <c r="L14" s="9"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="L14" s="34">
+        <v>3</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C15" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D15" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E15" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F15" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G15" s="8">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H15" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I15" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J15" s="8">
-        <v>0</v>
-      </c>
-      <c r="L15" s="9"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="L15" s="33">
+        <v>4</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C16" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D16" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E16" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F16" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G16" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H16" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I16" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J16" s="8">
-        <v>0</v>
-      </c>
-      <c r="L16" s="9"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="L16" s="34">
+        <v>5</v>
+      </c>
+      <c r="M16" s="9"/>
+      <c r="N16" s="10"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C17" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D17" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E17" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F17" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G17" s="8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H17" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I17" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J17" s="8">
-        <v>0</v>
-      </c>
-      <c r="L17" s="9"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="L17" s="33">
+        <v>6</v>
+      </c>
+      <c r="M17" s="9"/>
+      <c r="N17" s="10"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C18" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D18" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E18" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F18" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G18" s="8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H18" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I18" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J18" s="8">
-        <v>0</v>
-      </c>
-      <c r="L18" s="9"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="L18" s="34">
+        <v>7</v>
+      </c>
+      <c r="M18" s="9"/>
+      <c r="N18" s="10"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C19" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D19" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E19" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F19" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G19" s="8">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H19" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I19" s="8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J19" s="8">
-        <v>0</v>
-      </c>
-      <c r="L19" s="9"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="L19" s="33">
+        <v>8</v>
+      </c>
+      <c r="M19" s="9"/>
+      <c r="N19" s="10"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C20" s="8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D20" s="8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E20" s="8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F20" s="8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G20" s="8">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H20" s="8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I20" s="8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J20" s="8">
-        <v>0</v>
-      </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="11"/>
+        <v>11</v>
+      </c>
+      <c r="L20" s="34">
+        <v>9</v>
+      </c>
+      <c r="M20" s="9"/>
+      <c r="N20" s="10"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C21" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D21" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E21" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F21" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G21" s="8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H21" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I21" s="8">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J21" s="8">
-        <v>0</v>
-      </c>
-      <c r="L21" s="9"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="L21" s="33">
+        <v>10</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="10"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C22" s="8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D22" s="8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E22" s="8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F22" s="8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G22" s="8">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H22" s="8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I22" s="8">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J22" s="8">
-        <v>0</v>
-      </c>
-      <c r="L22" s="9"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="L22" s="34">
+        <v>11</v>
+      </c>
+      <c r="M22" s="9"/>
+      <c r="N22" s="10"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="8">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C23" s="8">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D23" s="8">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E23" s="8">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F23" s="8">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G23" s="8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H23" s="8">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I23" s="8">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J23" s="8">
-        <v>0</v>
-      </c>
-      <c r="L23" s="9"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="L23" s="33">
+        <v>12</v>
+      </c>
+      <c r="M23" s="9"/>
+      <c r="N23" s="10"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C24" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D24" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E24" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F24" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G24" s="8">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H24" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I24" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J24" s="8">
-        <v>0</v>
-      </c>
-      <c r="L24" s="9"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="11"/>
+        <v>15</v>
+      </c>
+      <c r="L24" s="34">
+        <v>13</v>
+      </c>
+      <c r="M24" s="9"/>
+      <c r="N24" s="10"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C25" s="8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D25" s="8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E25" s="8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F25" s="8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G25" s="8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H25" s="8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I25" s="8">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J25" s="8">
-        <v>0</v>
-      </c>
-      <c r="L25" s="9"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="L25" s="33">
+        <v>14</v>
+      </c>
+      <c r="M25" s="9"/>
+      <c r="N25" s="10"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B26" s="8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C26" s="8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D26" s="8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E26" s="8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F26" s="8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G26" s="8">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H26" s="8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="I26" s="8">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J26" s="8">
-        <v>0</v>
-      </c>
-      <c r="L26" s="9"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="L26" s="34">
+        <v>15</v>
+      </c>
+      <c r="M26" s="9"/>
+      <c r="N26" s="10"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="8">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C27" s="8">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D27" s="8">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E27" s="8">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F27" s="8">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G27" s="8">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H27" s="8">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I27" s="8">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J27" s="8">
-        <v>0</v>
-      </c>
-      <c r="L27" s="9"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="L27" s="33">
+        <v>16</v>
+      </c>
+      <c r="M27" s="9"/>
+      <c r="N27" s="10"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="8">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C28" s="8">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D28" s="8">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E28" s="8">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F28" s="8">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G28" s="8">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H28" s="8">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="I28" s="8">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="J28" s="8">
-        <v>0</v>
-      </c>
-      <c r="L28" s="9"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="11"/>
+        <v>19</v>
+      </c>
+      <c r="L28" s="34">
+        <v>17</v>
+      </c>
+      <c r="M28" s="9"/>
+      <c r="N28" s="10"/>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B29" s="8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C29" s="8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D29" s="8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E29" s="8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F29" s="8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G29" s="8">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="H29" s="8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I29" s="8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J29" s="8">
-        <v>0</v>
-      </c>
-      <c r="L29" s="9"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="11"/>
+        <v>20</v>
+      </c>
+      <c r="L29" s="33">
+        <v>18</v>
+      </c>
+      <c r="M29" s="9"/>
+      <c r="N29" s="10"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B30" s="8">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C30" s="8">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D30" s="8">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E30" s="8">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F30" s="8">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="G30" s="8">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="H30" s="8">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="I30" s="8">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J30" s="8">
-        <v>0</v>
-      </c>
-      <c r="L30" s="9"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="11"/>
+        <v>21</v>
+      </c>
+      <c r="L30" s="34">
+        <v>19</v>
+      </c>
+      <c r="M30" s="9"/>
+      <c r="N30" s="10"/>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C31" s="8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D31" s="8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E31" s="8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F31" s="8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G31" s="8">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H31" s="8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I31" s="8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J31" s="8">
-        <v>0</v>
-      </c>
-      <c r="L31" s="9"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="L31" s="33">
+        <v>20</v>
+      </c>
+      <c r="M31" s="9"/>
+      <c r="N31" s="10"/>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="8">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C32" s="8">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D32" s="8">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E32" s="8">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F32" s="8">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G32" s="8">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="H32" s="8">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I32" s="8">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J32" s="8">
-        <v>0</v>
-      </c>
-      <c r="L32" s="9"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="L32" s="34">
+        <v>21</v>
+      </c>
+      <c r="M32" s="9"/>
+      <c r="N32" s="10"/>
     </row>
     <row r="33" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B33" s="8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C33" s="8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D33" s="8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E33" s="8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F33" s="8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G33" s="8">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="H33" s="8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="I33" s="8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="J33" s="8">
-        <v>0</v>
-      </c>
-      <c r="L33" s="9"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="L33" s="33">
+        <v>22</v>
+      </c>
+      <c r="M33" s="9"/>
+      <c r="N33" s="10"/>
     </row>
     <row r="34" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B34" s="8">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C34" s="8">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D34" s="8">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E34" s="8">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F34" s="8">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G34" s="8">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="H34" s="8">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I34" s="8">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="J34" s="8">
-        <v>0</v>
-      </c>
-      <c r="L34" s="9"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="11">
+        <v>25</v>
+      </c>
+      <c r="L34" s="34">
+        <v>23</v>
+      </c>
+      <c r="M34" s="9"/>
+      <c r="N34" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="13">
+      <c r="B35" s="12">
         <f t="shared" ref="B35:J35" si="0">MAX(B11:B34)</f>
-        <v>0</v>
-      </c>
-      <c r="C35" s="13">
+        <v>25</v>
+      </c>
+      <c r="C35" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D35" s="13">
+        <v>25</v>
+      </c>
+      <c r="D35" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="14">
+        <v>25</v>
+      </c>
+      <c r="E35" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="13">
+        <v>25</v>
+      </c>
+      <c r="F35" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G35" s="13">
+        <v>25</v>
+      </c>
+      <c r="G35" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H35" s="14">
+        <v>33</v>
+      </c>
+      <c r="H35" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I35" s="14">
+        <v>25</v>
+      </c>
+      <c r="I35" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="14">
+        <v>25</v>
+      </c>
+      <c r="J35" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L35" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L35" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="M35" s="16">
+      <c r="M35" s="15">
         <f>MAX(M11:M34)</f>
         <v>0</v>
       </c>
-      <c r="N35" s="17"/>
+      <c r="N35" s="16"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="13">
+      <c r="B36" s="12">
         <f>AVERAGE(B11:B34)</f>
-        <v>0</v>
-      </c>
-      <c r="C36" s="13">
+        <v>13.5</v>
+      </c>
+      <c r="C36" s="12">
         <f t="shared" ref="C36:J36" si="1">AVERAGE(C11:C34)</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="13">
+        <v>13.5</v>
+      </c>
+      <c r="D36" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E36" s="14">
+        <v>13.5</v>
+      </c>
+      <c r="E36" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="13">
+        <v>13.5</v>
+      </c>
+      <c r="F36" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G36" s="13">
+        <v>13.5</v>
+      </c>
+      <c r="G36" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H36" s="14">
+        <v>21.5</v>
+      </c>
+      <c r="H36" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I36" s="14">
+        <v>13.5</v>
+      </c>
+      <c r="I36" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J36" s="14">
+        <v>13.5</v>
+      </c>
+      <c r="J36" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L36" s="15" t="s">
+        <v>13.5</v>
+      </c>
+      <c r="L36" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="M36" s="16" t="e">
+      <c r="M36" s="15" t="e">
         <f>AVERAGE(M11:M34)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="12">
         <f t="shared" ref="B37:J37" si="2">MIN(B11:B34)</f>
-        <v>0</v>
-      </c>
-      <c r="C37" s="13">
+        <v>2</v>
+      </c>
+      <c r="C37" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="D37" s="13">
+        <v>2</v>
+      </c>
+      <c r="D37" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E37" s="14">
+        <v>2</v>
+      </c>
+      <c r="E37" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="13">
+        <v>2</v>
+      </c>
+      <c r="F37" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G37" s="13">
+        <v>2</v>
+      </c>
+      <c r="G37" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H37" s="14">
+        <v>10</v>
+      </c>
+      <c r="H37" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I37" s="14">
+        <v>2</v>
+      </c>
+      <c r="I37" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="14">
+        <v>2</v>
+      </c>
+      <c r="J37" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L37" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L37" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="M37" s="16">
+      <c r="M37" s="15">
         <f>MIN(M11:M34)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="23"/>
-      <c r="L38" s="24"/>
-      <c r="M38" s="25"/>
+      <c r="A38" s="17"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="22"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="24"/>
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="18"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="23"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="29"/>
-      <c r="O39" s="29"/>
+      <c r="A39" s="17"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="22"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="28"/>
     </row>
     <row r="40" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I40" s="22"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="30"/>
-      <c r="N40" s="29"/>
+      <c r="I40" s="21"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="28"/>
     </row>
     <row r="41" spans="1:19" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D41" s="35" t="s">
+      <c r="D41" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="35"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
       <c r="J41" s="1"/>
-      <c r="M41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="29"/>
-      <c r="S41" s="29"/>
+      <c r="M41" s="29"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="29"/>
+      <c r="Q41" s="29"/>
+      <c r="R41" s="28"/>
+      <c r="S41" s="28"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A42" s="34" t="e" vm="1">
+      <c r="A42" s="36" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="36" t="str">
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="38" t="str">
         <f>+D2</f>
         <v xml:space="preserve">Coordinación de Operación De Explotación </v>
       </c>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="K42" s="51" t="e" vm="2">
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="K42" s="40" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="L42" s="51"/>
-      <c r="M42" s="51"/>
-      <c r="N42" s="53"/>
+      <c r="L42" s="40"/>
+      <c r="M42" s="40"/>
+      <c r="N42" s="2"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34" t="str">
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36" t="str">
         <f>+D3</f>
         <v>Contrato 425014809</v>
       </c>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="K43" s="51"/>
-      <c r="L43" s="51"/>
-      <c r="M43" s="51"/>
-      <c r="N43" s="53"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="K43" s="40"/>
+      <c r="L43" s="40"/>
+      <c r="M43" s="40"/>
+      <c r="N43" s="2"/>
     </row>
     <row r="44" spans="1:19" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="52" t="str">
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="39" t="str">
         <f>+D4</f>
         <v>Pozo IRIDE 5108</v>
       </c>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="53"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="40"/>
+      <c r="N44" s="2"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D45" s="34" t="str">
+      <c r="D45" s="36" t="str">
         <f>+D5</f>
         <v>Supervisor Ing. Angel Adrian Castro Acosta.</v>
       </c>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="34"/>
-      <c r="I45" s="34"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
     </row>
     <row r="46" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E46" t="str">
+      <c r="D46" s="35" t="str">
         <f>+D6</f>
         <v>Activo De Extraccion Samaria Luna</v>
       </c>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
     </row>
     <row r="47" spans="1:19" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="48" t="s">
+      <c r="A47" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="49"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="49"/>
-      <c r="I47" s="49"/>
-      <c r="J47" s="49"/>
-      <c r="K47" s="49"/>
-      <c r="L47" s="50"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="53"/>
+      <c r="L47" s="54"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
-      <c r="J48" s="38"/>
-      <c r="K48" s="38"/>
-      <c r="L48" s="39"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="42"/>
+      <c r="L48" s="43"/>
     </row>
     <row r="49" spans="1:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="40"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="41"/>
-      <c r="H49" s="41"/>
-      <c r="I49" s="41"/>
-      <c r="J49" s="41"/>
-      <c r="K49" s="41"/>
-      <c r="L49" s="42"/>
+      <c r="A49" s="44"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="45"/>
+      <c r="L49" s="46"/>
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="31"/>
-      <c r="L50" s="31"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="32"/>
+      <c r="K50" s="30"/>
+      <c r="L50" s="30"/>
     </row>
     <row r="51" spans="1:12" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="23">
     <mergeCell ref="A42:C44"/>
     <mergeCell ref="K4:M6"/>
     <mergeCell ref="K42:M44"/>
@@ -2396,6 +2985,7 @@
     <mergeCell ref="D44:I44"/>
     <mergeCell ref="D45:I45"/>
     <mergeCell ref="A47:L47"/>
+    <mergeCell ref="D46:I46"/>
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="D2:I2"/>

</xml_diff>